<commit_message>
Cleaned up the behavior logic, behavior is now output
</commit_message>
<xml_diff>
--- a/Keycorder GUI/Keycorder GUI/Config.xlsx
+++ b/Keycorder GUI/Keycorder GUI/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Key-Corder\Keycorder GUI\Keycorder GUI\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\Key-Corder\Keycorder GUI\Keycorder GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6353F350-7778-49CC-82C6-C7EAE4E52F12}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29610" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29610" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="94">
   <si>
     <t>Key</t>
   </si>
@@ -180,9 +181,6 @@
   </si>
   <si>
     <t>Behavior</t>
-  </si>
-  <si>
-    <t>TANG</t>
   </si>
   <si>
     <t>ATTN</t>
@@ -314,7 +312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -659,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,9 +693,6 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
       <c r="D2">
         <v>45</v>
       </c>
@@ -716,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -733,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -750,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -764,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -778,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -792,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -806,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -820,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -834,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -848,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -862,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -876,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -890,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
@@ -904,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -918,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -932,7 +927,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
@@ -946,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -960,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
@@ -974,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -988,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
@@ -1002,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
@@ -1016,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -1030,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
@@ -1044,7 +1039,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
@@ -1058,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
@@ -1072,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -1086,7 +1081,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -1100,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -1114,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -1128,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -1142,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -1156,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -1170,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -1184,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -1198,7 +1193,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
@@ -1212,7 +1207,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1226,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1240,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
@@ -1254,7 +1249,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
@@ -1268,7 +1263,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F42" t="s">
         <v>45</v>
@@ -1282,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
         <v>46</v>
@@ -1296,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
         <v>49</v>
@@ -1310,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
         <v>47</v>
@@ -1324,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F46" t="s">
         <v>48</v>
@@ -1332,10 +1327,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$E$2:$E$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6 A9:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6 A9:A1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$F:$F</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Set save dialog filter. Updated EEPlus package.
</commit_message>
<xml_diff>
--- a/Keycorder GUI/Keycorder GUI/Config.xlsx
+++ b/Keycorder GUI/Keycorder GUI/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\Key-Corder\Keycorder GUI\Keycorder GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.borgen\OneDrive for Business\Migrated-S-Drive\PFDP\Keycorder\Keycorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6353F350-7778-49CC-82C6-C7EAE4E52F12}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29610" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29616" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
   <si>
     <t>Key</t>
   </si>
@@ -201,9 +200,6 @@
     <t>PRAISE</t>
   </si>
   <si>
-    <t>EMESEIS</t>
-  </si>
-  <si>
     <t>GAG</t>
   </si>
   <si>
@@ -216,15 +212,6 @@
     <t>SIB</t>
   </si>
   <si>
-    <t>RP BITE</t>
-  </si>
-  <si>
-    <t>RP DRINK</t>
-  </si>
-  <si>
-    <t>BITE ACC</t>
-  </si>
-  <si>
     <t>NEG VOC</t>
   </si>
   <si>
@@ -234,85 +221,106 @@
     <t>IMB</t>
   </si>
   <si>
-    <t>IND BITE</t>
-  </si>
-  <si>
-    <t>BITE MC</t>
-  </si>
-  <si>
-    <t>PAC K</t>
-  </si>
-  <si>
     <t>LAT ACC</t>
   </si>
   <si>
     <t>LAT MC</t>
   </si>
   <si>
-    <t>DUR1</t>
-  </si>
-  <si>
-    <t>PHYSG</t>
-  </si>
-  <si>
-    <t>BPRES</t>
-  </si>
-  <si>
-    <t>BABS</t>
-  </si>
-  <si>
-    <t>BITEACC</t>
-  </si>
-  <si>
     <t>NODATA</t>
   </si>
   <si>
-    <t>ACC</t>
-  </si>
-  <si>
-    <t>DRINK</t>
-  </si>
-  <si>
-    <t>BITEABS</t>
-  </si>
-  <si>
-    <t>IDRINK</t>
-  </si>
-  <si>
-    <t>MDRINK</t>
-  </si>
-  <si>
-    <t>ADRINK</t>
-  </si>
-  <si>
-    <t>FPRO</t>
-  </si>
-  <si>
-    <t>JPRO</t>
-  </si>
-  <si>
-    <t>CPRO</t>
-  </si>
-  <si>
-    <t>BPRO</t>
-  </si>
-  <si>
-    <t>DC1</t>
-  </si>
-  <si>
-    <t>ND1</t>
-  </si>
-  <si>
-    <t>DPRO</t>
-  </si>
-  <si>
-    <t>DC2</t>
+    <t>TANG</t>
+  </si>
+  <si>
+    <t>BLOCKY</t>
+  </si>
+  <si>
+    <t>BLOCKN</t>
+  </si>
+  <si>
+    <t>EMESIS</t>
+  </si>
+  <si>
+    <t>NO DATA</t>
+  </si>
+  <si>
+    <t>PACK</t>
+  </si>
+  <si>
+    <t>JAW P</t>
+  </si>
+  <si>
+    <t>CHIN P</t>
+  </si>
+  <si>
+    <t>FING P</t>
+  </si>
+  <si>
+    <t>PHYS G</t>
+  </si>
+  <si>
+    <t>RP SOL</t>
+  </si>
+  <si>
+    <t>RP SACC</t>
+  </si>
+  <si>
+    <t>RP LIQ</t>
+  </si>
+  <si>
+    <t>RP LACC</t>
+  </si>
+  <si>
+    <t>LIQ ACC</t>
+  </si>
+  <si>
+    <t>LIQ PRES</t>
+  </si>
+  <si>
+    <t>SOL ACC</t>
+  </si>
+  <si>
+    <t>SOL PRES</t>
+  </si>
+  <si>
+    <t>SOL ABS</t>
+  </si>
+  <si>
+    <t>SOL PRO</t>
+  </si>
+  <si>
+    <t>IND LIQ</t>
+  </si>
+  <si>
+    <t>IND SOL</t>
+  </si>
+  <si>
+    <t>LIQ MC</t>
+  </si>
+  <si>
+    <t>SOL MC</t>
+  </si>
+  <si>
+    <t>LIQ ABS</t>
+  </si>
+  <si>
+    <t>LIQ PRO</t>
+  </si>
+  <si>
+    <t>DUMMY 1</t>
+  </si>
+  <si>
+    <t>DUM DUR</t>
+  </si>
+  <si>
+    <t>CORRECT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -657,22 +665,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,13 +695,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
       <c r="D2">
         <v>45</v>
       </c>
@@ -703,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -720,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -737,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -751,21 +763,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -773,13 +785,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -787,13 +799,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -807,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -815,13 +827,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -829,13 +841,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -843,13 +855,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -857,13 +869,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -877,7 +889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -891,7 +903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -899,41 +911,41 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -941,13 +953,13 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -955,13 +967,13 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -969,13 +981,13 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -983,13 +995,13 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -997,13 +1009,13 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1011,13 +1023,13 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1025,13 +1037,13 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1039,27 +1051,27 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1067,13 +1079,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1081,13 +1093,13 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1095,13 +1107,13 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1109,13 +1121,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1123,13 +1135,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1137,13 +1149,13 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1151,27 +1163,27 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1179,13 +1191,13 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -1193,13 +1205,13 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1207,13 +1219,13 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1221,13 +1233,13 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1235,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1249,27 +1261,27 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1277,13 +1289,13 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F43" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1291,13 +1303,13 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1305,21 +1317,21 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F46" t="s">
         <v>48</v>
@@ -1327,10 +1339,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>$E$2:$E$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6 A9:A1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6 A9:A1048576">
       <formula1>$F:$F</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>